<commit_message>
first version dellstore completed
</commit_message>
<xml_diff>
--- a/dellstore_sourcetotarget_map..xlsx
+++ b/dellstore_sourcetotarget_map..xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="155">
   <si>
     <t>inventory</t>
   </si>
@@ -428,6 +428,60 @@
   </si>
   <si>
     <t>LOAD_DATE</t>
+  </si>
+  <si>
+    <t>price_mean</t>
+  </si>
+  <si>
+    <t>price_max</t>
+  </si>
+  <si>
+    <t>price_min</t>
+  </si>
+  <si>
+    <t>price_median</t>
+  </si>
+  <si>
+    <t>total_sales</t>
+  </si>
+  <si>
+    <t>median of all prices bought</t>
+  </si>
+  <si>
+    <t>maximum of all prices</t>
+  </si>
+  <si>
+    <t>max_ordersize</t>
+  </si>
+  <si>
+    <t>minimum of prirces bought</t>
+  </si>
+  <si>
+    <t>avg of all prices bought</t>
+  </si>
+  <si>
+    <t>total sales (incl. Taxes)</t>
+  </si>
+  <si>
+    <t>total number of orders</t>
+  </si>
+  <si>
+    <t>order count</t>
+  </si>
+  <si>
+    <t>max_quantity_per_order</t>
+  </si>
+  <si>
+    <t>CUST_STATS</t>
+  </si>
+  <si>
+    <t>number of lines in the order with the most lines</t>
+  </si>
+  <si>
+    <t>maximum total quantity bought in one order</t>
+  </si>
+  <si>
+    <t>surrogate key of customer</t>
   </si>
 </sst>
 </file>
@@ -1385,15 +1439,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
     <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.36328125" customWidth="1"/>
@@ -2019,7 +2074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>135</v>
       </c>
@@ -2028,6 +2083,132 @@
       </c>
       <c r="C49" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>